<commit_message>
Merged PR 51109: Added VerifyGlobalSearchTest, Updated GoToSpecificInboxTest, Updated inbox te...
Added VerifyGlobalSearchTest, Updated GoToSpecificInboxTest, Updated inbox test data.

Related work items: #252664, #523300, #523784, #523788
</commit_message>
<xml_diff>
--- a/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DVV/InboxData.xlsx
+++ b/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DVV/InboxData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\EnterpriseUX.Automation\West.EnterpriseUX.Automation\MobileAutomationCrossPlatform\TestData\UAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC581E0-8FB0-4FFA-A4EC-EB763D3B901E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D694609-DCD5-482F-B0D2-3B8951F38235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Function</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Inbox</t>
   </si>
   <si>
-    <t>Inbound</t>
-  </si>
-  <si>
-    <t>Purchase Orders</t>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>Customer Success</t>
+  </si>
+  <si>
+    <t>Sales Orders</t>
+  </si>
+  <si>
+    <t>SearchRecord</t>
+  </si>
+  <si>
+    <t>ZOR</t>
   </si>
 </sst>
 </file>
@@ -354,33 +360,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>